<commit_message>
Made django models and made admin.register
</commit_message>
<xml_diff>
--- a/Users/1048928261/Base.xlsx
+++ b/Users/1048928261/Base.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
   <si>
     <t>Имя</t>
   </si>
@@ -629,6 +629,772 @@
   </si>
   <si>
     <t>8-978-766-90-06</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">НОВИКОВ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Артем Владимирович</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-600-69-45</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">МЫШАК </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>С</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">ергей Васильевич </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>8-978-792-86-14 – доп.</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-857-13-30</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ГЕРАСИМЧУК </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Дмитрий Николаевич</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-100-15-70</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">НАЗАРОВА </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Маргарита Владимировна</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-91872-82</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">БОНДАРЧУК </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Александр Сергеевич</t>
+    </r>
+  </si>
+  <si>
+    <t>8-913-077-08-11</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ТАРАСЕНКО </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Борис Олегович</t>
+    </r>
+  </si>
+  <si>
+    <t>8-928-463-70-10</t>
+  </si>
+  <si>
+    <t>Петелин Михаил Александрович</t>
+  </si>
+  <si>
+    <t>СОЛОДОВНИКОВ Сергей Иванович</t>
+  </si>
+  <si>
+    <t>8-978-563-21-03</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">НАЗАРОВ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Илья Михайлович</t>
+    </r>
+  </si>
+  <si>
+    <t>8-910-146-02-17</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">МАКУШЕНКО </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Алексей Юрьевич</t>
+    </r>
+  </si>
+  <si>
+    <t>8-988-392-88-87</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ДИЕСПЕРОВ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Григорий Иванович</t>
+    </r>
+  </si>
+  <si>
+    <t>8-910-302-88-04</t>
+  </si>
+  <si>
+    <t>Проплеткин Андрей</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>САЗОНОВ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Александр Николаевич</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-738-40-83</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ЛАЗАРЕВ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Назар Валерьевич</t>
+    </r>
+  </si>
+  <si>
+    <t>8-910-244-15-72</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ГЕЛЕВИЧ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Евгений Владимирович</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-080-54-11</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ЦУКАНОВ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Антон Андреевич</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-558-62-49</t>
+  </si>
+  <si>
+    <t>Родион Голенков</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">КУРМАШОВ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Виталий Вадимович</t>
+    </r>
+  </si>
+  <si>
+    <t>8-987-654-55-06</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">КУТОВОЙ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Евгений Александрович</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-214-98-38</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">МИХАЙЛЕНКО </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Даниил Эрнестович</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-728-43-78</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ЖАШКОВ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Роман Александрович</t>
+    </r>
+  </si>
+  <si>
+    <t>8-980-546-40-14</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ДУВАНОВ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Алексей Алексеевич</t>
+    </r>
+  </si>
+  <si>
+    <t>8-960-119-50-95</t>
+  </si>
+  <si>
+    <t>Семенов Саша</t>
+  </si>
+  <si>
+    <t>Ивлев Никита</t>
+  </si>
+  <si>
+    <t>Краснов Артем</t>
+  </si>
+  <si>
+    <t>Толстолыткин Влад</t>
+  </si>
+  <si>
+    <t>Олейник Света</t>
+  </si>
+  <si>
+    <t>Леонидова Ксюша</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ДМИТРИЕВ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Роман Юрьевич</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-744-70-02</t>
+  </si>
+  <si>
+    <t>Петренко Игнат</t>
+  </si>
+  <si>
+    <t>Кривко Дима</t>
+  </si>
+  <si>
+    <t>Олеся степина</t>
+  </si>
+  <si>
+    <t>Токарев Илья</t>
+  </si>
+  <si>
+    <t>Благий Вова</t>
+  </si>
+  <si>
+    <t>Дима Данильченко</t>
+  </si>
+  <si>
+    <t>КУдрин Илья</t>
+  </si>
+  <si>
+    <t>Марк Сучков</t>
+  </si>
+  <si>
+    <t>Олег Романов</t>
+  </si>
+  <si>
+    <t>Разумников Илья</t>
+  </si>
+  <si>
+    <t>Даня Григорян</t>
+  </si>
+  <si>
+    <t>Петров Антон</t>
+  </si>
+  <si>
+    <t>Ваня Санников</t>
+  </si>
+  <si>
+    <t>Паша Машаров</t>
+  </si>
+  <si>
+    <t>Леонтьев Артем</t>
+  </si>
+  <si>
+    <t>МАксим Трохачев</t>
+  </si>
+  <si>
+    <t>Тутов Станислав</t>
+  </si>
+  <si>
+    <t>Давыдов Вадим</t>
+  </si>
+  <si>
+    <t>Земцов Артем</t>
+  </si>
+  <si>
+    <t>Настя Приставка</t>
+  </si>
+  <si>
+    <t>Михалев Паша</t>
+  </si>
+  <si>
+    <t>Миша Блинков</t>
+  </si>
+  <si>
+    <t>Резниченко Олег</t>
+  </si>
+  <si>
+    <t>Курилова Настя</t>
+  </si>
+  <si>
+    <t>Кабанов Саша</t>
+  </si>
+  <si>
+    <t>Настя Блинкова</t>
+  </si>
+  <si>
+    <t>Бебенин Борис Александрович</t>
+  </si>
+  <si>
+    <t>Антон Клещев</t>
+  </si>
+  <si>
+    <t>Игнашин Максим</t>
+  </si>
+  <si>
+    <t>Лаптев Сергей</t>
+  </si>
+  <si>
+    <t>Шестов Стас</t>
+  </si>
+  <si>
+    <t>Растворов Кирилл</t>
+  </si>
+  <si>
+    <t>Новосело Дима</t>
+  </si>
+  <si>
+    <t>Мирзаева Элина</t>
+  </si>
+  <si>
+    <t>Кривенцов Илья</t>
+  </si>
+  <si>
+    <t>Баранов Олег</t>
+  </si>
+  <si>
+    <t>Костя Анисимов</t>
+  </si>
+  <si>
+    <t>Алексей Орлов</t>
+  </si>
+  <si>
+    <t>Лера Садовникова</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">САДОВНИКОВ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Дмитрий Васильевич</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-543-26-64</t>
+  </si>
+  <si>
+    <t>Лера Жена</t>
+  </si>
+  <si>
+    <t>+79782487684</t>
+  </si>
+  <si>
+    <t>Астапкович Дима</t>
+  </si>
+  <si>
+    <t>Евгений Надточеев</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ЯКОВЛЕВ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Константин</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Николаевич</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-296-52-77</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ДУДНИКОВ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Андрей Николаевич</t>
+    </r>
+  </si>
+  <si>
+    <t>8-910-744-87-55</t>
+  </si>
+  <si>
+    <t>Даша Сестра</t>
+  </si>
+  <si>
+    <t>Дима Павлов</t>
+  </si>
+  <si>
+    <t>Лиза</t>
+  </si>
+  <si>
+    <t>Ростик</t>
   </si>
 </sst>
 </file>
@@ -638,23 +1404,16 @@
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_-* #\ ##0_-;\-* #\ ##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #\ ##0\ &quot;₽&quot;_-;\-* #\ ##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #\ ##0.00\ &quot;₽&quot;_-;\-* #\ ##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="[$-419]d\ mmmm\ yyyy\ &quot;r.&quot;;@"/>
-    <numFmt numFmtId="180" formatCode="_-* #\ ##0.00_-;\-* #\ ##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #\ ##0.00_-;\-* #\ ##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #\ ##0.00\ &quot;₽&quot;_-;\-* #\ ##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="[$-419]d\ mmmm\ yyyy\ &quot;r.&quot;;@"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -666,7 +1425,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -679,8 +1438,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -691,30 +1458,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -734,8 +1477,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -774,6 +1532,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -788,8 +1553,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -801,6 +1567,13 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial Narrow"/>
@@ -822,7 +1595,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -834,13 +1625,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -852,31 +1691,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -894,19 +1715,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -918,25 +1751,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -948,61 +1769,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1031,17 +1804,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1049,8 +1816,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1105,11 +1872,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1131,52 +1904,55 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1185,94 +1961,91 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1280,10 +2053,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1605,8 +2379,8 @@
   <sheetPr/>
   <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1641,7 +2415,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3">
-        <v>19455</v>
+        <v>19377</v>
       </c>
       <c r="C3" s="4"/>
     </row>
@@ -1650,7 +2424,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>24202</v>
+        <v>24143</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -1670,7 +2444,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="3">
-        <v>24933</v>
+        <v>24937</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>9</v>
@@ -1942,393 +2716,753 @@
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="2"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="4"/>
+      <c r="A32" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="3">
+        <v>31824</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="4"/>
+      <c r="A33" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="3">
+        <v>32034</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="2"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="4"/>
+      <c r="A34" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="3">
+        <v>32045</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="2"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="4"/>
+      <c r="A35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="3">
+        <v>32612</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="2"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="4"/>
+      <c r="A36" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="3">
+        <v>32767</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="2"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="4"/>
+      <c r="A37" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="3">
+        <v>32767</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="2"/>
-      <c r="B38" s="3"/>
+      <c r="A38" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="3">
+        <v>33121</v>
+      </c>
       <c r="C38" s="4"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="2"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="4"/>
+      <c r="A39" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="3">
+        <v>33295</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="2"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="4"/>
+      <c r="A40" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="3">
+        <v>33476</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="2"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="4"/>
+      <c r="A41" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="3">
+        <v>33540</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="2"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="4"/>
+      <c r="A42" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" s="3">
+        <v>34063</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="2"/>
-      <c r="B43" s="3"/>
+      <c r="A43" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" s="3">
+        <v>34381</v>
+      </c>
       <c r="C43" s="4"/>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="2"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="4"/>
+      <c r="A44" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" s="3">
+        <v>34451</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="2"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="4"/>
+      <c r="A45" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" s="3">
+        <v>34505</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="2"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="4"/>
+      <c r="A46" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" s="3">
+        <v>34550</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="2"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="4"/>
+      <c r="A47" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47" s="3">
+        <v>34710</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="2"/>
-      <c r="B48" s="3"/>
+      <c r="A48" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" s="3">
+        <v>34735</v>
+      </c>
       <c r="C48" s="4"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="2"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="4"/>
+      <c r="A49" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="3">
+        <v>34834</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="2"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="4"/>
+      <c r="A50" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="3">
+        <v>34837</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="2"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="4"/>
+      <c r="A51" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B51" s="3">
+        <v>34856</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="2"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="4"/>
+      <c r="A52" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" s="3">
+        <v>34930</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="2"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="4"/>
+      <c r="A53" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B53" s="3">
+        <v>34997</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="2"/>
-      <c r="B54" s="3"/>
+      <c r="A54" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" s="3">
+        <v>35081</v>
+      </c>
       <c r="C54" s="4"/>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="2"/>
-      <c r="B55" s="3"/>
+      <c r="A55" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B55" s="3">
+        <v>35082</v>
+      </c>
       <c r="C55" s="4"/>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="2"/>
-      <c r="B56" s="3"/>
+      <c r="A56" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" s="3">
+        <v>35102</v>
+      </c>
       <c r="C56" s="4"/>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="2"/>
-      <c r="B57" s="3"/>
+      <c r="A57" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B57" s="3">
+        <v>35102</v>
+      </c>
       <c r="C57" s="4"/>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="2"/>
-      <c r="B58" s="3"/>
+      <c r="A58" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B58" s="3">
+        <v>35103</v>
+      </c>
       <c r="C58" s="4"/>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="2"/>
-      <c r="B59" s="3"/>
+      <c r="A59" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B59" s="3">
+        <v>35103</v>
+      </c>
       <c r="C59" s="4"/>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="2"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="4"/>
+      <c r="A60" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B60" s="3">
+        <v>35110</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="2"/>
-      <c r="B61" s="3"/>
+      <c r="A61" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B61" s="3">
+        <v>35121</v>
+      </c>
       <c r="C61" s="4"/>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="2"/>
-      <c r="B62" s="3"/>
+      <c r="A62" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B62" s="3">
+        <v>35143</v>
+      </c>
       <c r="C62" s="4"/>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="2"/>
-      <c r="B63" s="3"/>
+      <c r="A63" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B63" s="3">
+        <v>35149</v>
+      </c>
       <c r="C63" s="4"/>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="2"/>
-      <c r="B64" s="3"/>
+      <c r="A64" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B64" s="3">
+        <v>35153</v>
+      </c>
       <c r="C64" s="4"/>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="2"/>
-      <c r="B65" s="3"/>
+      <c r="A65" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B65" s="3">
+        <v>35154</v>
+      </c>
       <c r="C65" s="4"/>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="2"/>
-      <c r="B66" s="3"/>
+      <c r="A66" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B66" s="3">
+        <v>35156</v>
+      </c>
       <c r="C66" s="4"/>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="2"/>
-      <c r="B67" s="3"/>
+      <c r="A67" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B67" s="3">
+        <v>35164</v>
+      </c>
       <c r="C67" s="4"/>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="2"/>
-      <c r="B68" s="3"/>
+      <c r="A68" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B68" s="3">
+        <v>35173</v>
+      </c>
       <c r="C68" s="4"/>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="2"/>
-      <c r="B69" s="3"/>
+      <c r="A69" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B69" s="3">
+        <v>35181</v>
+      </c>
       <c r="C69" s="4"/>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="2"/>
-      <c r="B70" s="3"/>
+      <c r="A70" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B70" s="3">
+        <v>35186</v>
+      </c>
       <c r="C70" s="4"/>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="2"/>
-      <c r="B71" s="3"/>
+      <c r="A71" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B71" s="3">
+        <v>35195</v>
+      </c>
       <c r="C71" s="4"/>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="2"/>
-      <c r="B72" s="3"/>
+      <c r="A72" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B72" s="3">
+        <v>35213</v>
+      </c>
       <c r="C72" s="4"/>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="2"/>
-      <c r="B73" s="3"/>
+      <c r="A73" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B73" s="3">
+        <v>35225</v>
+      </c>
       <c r="C73" s="4"/>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="2"/>
-      <c r="B74" s="3"/>
+      <c r="A74" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B74" s="3">
+        <v>35243</v>
+      </c>
       <c r="C74" s="4"/>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="2"/>
-      <c r="B75" s="3"/>
+      <c r="A75" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B75" s="3">
+        <v>35252</v>
+      </c>
       <c r="C75" s="4"/>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="2"/>
-      <c r="B76" s="3"/>
+      <c r="A76" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B76" s="3">
+        <v>35264</v>
+      </c>
       <c r="C76" s="4"/>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="2"/>
-      <c r="B77" s="3"/>
+      <c r="A77" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B77" s="3">
+        <v>35264</v>
+      </c>
       <c r="C77" s="4"/>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="2"/>
-      <c r="B78" s="3"/>
+      <c r="A78" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B78" s="3">
+        <v>35265</v>
+      </c>
       <c r="C78" s="4"/>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="2"/>
-      <c r="B79" s="3"/>
+      <c r="A79" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B79" s="3">
+        <v>35268</v>
+      </c>
       <c r="C79" s="4"/>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" s="2"/>
-      <c r="B80" s="3"/>
+      <c r="A80" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B80" s="3">
+        <v>35270</v>
+      </c>
       <c r="C80" s="4"/>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="2"/>
-      <c r="B81" s="3"/>
+      <c r="A81" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B81" s="3">
+        <v>35307</v>
+      </c>
       <c r="C81" s="4"/>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="2"/>
-      <c r="B82" s="3"/>
+      <c r="A82" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B82" s="3">
+        <v>35312</v>
+      </c>
       <c r="C82" s="4"/>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="2"/>
-      <c r="B83" s="3"/>
+      <c r="A83" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B83" s="3">
+        <v>35317</v>
+      </c>
       <c r="C83" s="4"/>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" s="2"/>
-      <c r="B84" s="3"/>
+      <c r="A84" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B84" s="3">
+        <v>35331</v>
+      </c>
       <c r="C84" s="4"/>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="2"/>
-      <c r="B85" s="3"/>
+      <c r="A85" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B85" s="3">
+        <v>35334</v>
+      </c>
       <c r="C85" s="4"/>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="2"/>
-      <c r="B86" s="3"/>
+      <c r="A86" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B86" s="3">
+        <v>35338</v>
+      </c>
       <c r="C86" s="4"/>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="2"/>
-      <c r="B87" s="3"/>
+      <c r="A87" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B87" s="3">
+        <v>35339</v>
+      </c>
       <c r="C87" s="4"/>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="2"/>
-      <c r="B88" s="3"/>
+      <c r="A88" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B88" s="3">
+        <v>35339</v>
+      </c>
       <c r="C88" s="4"/>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="2"/>
-      <c r="B89" s="3"/>
+      <c r="A89" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B89" s="3">
+        <v>35344</v>
+      </c>
       <c r="C89" s="4"/>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" s="2"/>
-      <c r="B90" s="3"/>
+      <c r="A90" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B90" s="3">
+        <v>35345</v>
+      </c>
       <c r="C90" s="4"/>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="2"/>
-      <c r="B91" s="3"/>
+      <c r="A91" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B91" s="3">
+        <v>35360</v>
+      </c>
       <c r="C91" s="4"/>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" s="2"/>
-      <c r="B92" s="3"/>
+      <c r="A92" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B92" s="3">
+        <v>35374</v>
+      </c>
       <c r="C92" s="4"/>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="2"/>
-      <c r="B93" s="3"/>
+      <c r="A93" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B93" s="3">
+        <v>35376</v>
+      </c>
       <c r="C93" s="4"/>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="2"/>
-      <c r="B94" s="3"/>
+      <c r="A94" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B94" s="3">
+        <v>35386</v>
+      </c>
       <c r="C94" s="4"/>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="2"/>
-      <c r="B95" s="3"/>
+      <c r="A95" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B95" s="3">
+        <v>35401</v>
+      </c>
       <c r="C95" s="4"/>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="2"/>
-      <c r="B96" s="3"/>
+      <c r="A96" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B96" s="3">
+        <v>35417</v>
+      </c>
       <c r="C96" s="4"/>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="2"/>
-      <c r="B97" s="3"/>
+      <c r="A97" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B97" s="3">
+        <v>35440</v>
+      </c>
       <c r="C97" s="2"/>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="2"/>
-      <c r="B98" s="3"/>
+      <c r="A98" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B98" s="3">
+        <v>35453</v>
+      </c>
       <c r="C98" s="4"/>
     </row>
     <row r="99" spans="1:3">
-      <c r="A99" s="2"/>
-      <c r="B99" s="3"/>
+      <c r="A99" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B99" s="3">
+        <v>35463</v>
+      </c>
       <c r="C99" s="4"/>
     </row>
     <row r="100" spans="1:3">
-      <c r="A100" s="2"/>
-      <c r="B100" s="3"/>
-      <c r="C100" s="4"/>
+      <c r="A100" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B100" s="3">
+        <v>35545</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="101" spans="1:3">
-      <c r="A101" s="2"/>
-      <c r="B101" s="3"/>
-      <c r="C101" s="4"/>
+      <c r="A101" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B101" s="3">
+        <v>35601</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="102" spans="1:3">
-      <c r="A102" s="2"/>
-      <c r="B102" s="3"/>
+      <c r="A102" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B102" s="3">
+        <v>35643</v>
+      </c>
       <c r="C102" s="4"/>
     </row>
     <row r="103" spans="1:3">
-      <c r="A103" s="2"/>
-      <c r="B103" s="3"/>
+      <c r="A103" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B103" s="3">
+        <v>35805</v>
+      </c>
       <c r="C103" s="4"/>
     </row>
     <row r="104" spans="1:3">
-      <c r="A104" s="2"/>
-      <c r="B104" s="3"/>
-      <c r="C104" s="4"/>
+      <c r="A104" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B104" s="3">
+        <v>35845</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="105" spans="1:3">
-      <c r="A105" s="2"/>
-      <c r="B105" s="3"/>
-      <c r="C105" s="4"/>
+      <c r="A105" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B105" s="3">
+        <v>35955</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="106" spans="1:3">
-      <c r="A106" s="2"/>
-      <c r="B106" s="3"/>
+      <c r="A106" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B106" s="3">
+        <v>36741</v>
+      </c>
       <c r="C106" s="4"/>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" s="2"/>
-      <c r="B107" s="3"/>
+      <c r="A107" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B107" s="3">
+        <v>36836</v>
+      </c>
       <c r="C107" s="4"/>
     </row>
     <row r="108" spans="1:3">
-      <c r="A108" s="2"/>
-      <c r="B108" s="3"/>
+      <c r="A108" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B108" s="3">
+        <v>39597</v>
+      </c>
       <c r="C108" s="4"/>
     </row>
     <row r="109" spans="1:3">
-      <c r="A109" s="2"/>
-      <c r="B109" s="3"/>
+      <c r="A109" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B109" s="3">
+        <v>40210</v>
+      </c>
       <c r="C109" s="4"/>
     </row>
     <row r="110" spans="2:3">

</xml_diff>

<commit_message>
Made it working with django and full functionality
</commit_message>
<xml_diff>
--- a/Users/1048928261/Base.xlsx
+++ b/Users/1048928261/Base.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
   <si>
     <t>Имя</t>
   </si>
@@ -629,6 +629,772 @@
   </si>
   <si>
     <t>8-978-766-90-06</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">НОВИКОВ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Артем Владимирович</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-600-69-45</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">МЫШАК </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>С</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">ергей Васильевич </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>8-978-792-86-14 – доп.</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-857-13-30</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ГЕРАСИМЧУК </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Дмитрий Николаевич</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-100-15-70</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">НАЗАРОВА </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Маргарита Владимировна</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-91872-82</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">БОНДАРЧУК </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Александр Сергеевич</t>
+    </r>
+  </si>
+  <si>
+    <t>8-913-077-08-11</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ТАРАСЕНКО </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Борис Олегович</t>
+    </r>
+  </si>
+  <si>
+    <t>8-928-463-70-10</t>
+  </si>
+  <si>
+    <t>Петелин Михаил Александрович</t>
+  </si>
+  <si>
+    <t>СОЛОДОВНИКОВ Сергей Иванович</t>
+  </si>
+  <si>
+    <t>8-978-563-21-03</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">НАЗАРОВ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Илья Михайлович</t>
+    </r>
+  </si>
+  <si>
+    <t>8-910-146-02-17</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">МАКУШЕНКО </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Алексей Юрьевич</t>
+    </r>
+  </si>
+  <si>
+    <t>8-988-392-88-87</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ДИЕСПЕРОВ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Григорий Иванович</t>
+    </r>
+  </si>
+  <si>
+    <t>8-910-302-88-04</t>
+  </si>
+  <si>
+    <t>Проплеткин Андрей</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>САЗОНОВ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Александр Николаевич</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-738-40-83</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ЛАЗАРЕВ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Назар Валерьевич</t>
+    </r>
+  </si>
+  <si>
+    <t>8-910-244-15-72</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ГЕЛЕВИЧ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Евгений Владимирович</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-080-54-11</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ЦУКАНОВ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Антон Андреевич</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-558-62-49</t>
+  </si>
+  <si>
+    <t>Родион Голенков</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">КУРМАШОВ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Виталий Вадимович</t>
+    </r>
+  </si>
+  <si>
+    <t>8-987-654-55-06</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">КУТОВОЙ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Евгений Александрович</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-214-98-38</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">МИХАЙЛЕНКО </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Даниил Эрнестович</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-728-43-78</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ЖАШКОВ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Роман Александрович</t>
+    </r>
+  </si>
+  <si>
+    <t>8-980-546-40-14</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ДУВАНОВ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Алексей Алексеевич</t>
+    </r>
+  </si>
+  <si>
+    <t>8-960-119-50-95</t>
+  </si>
+  <si>
+    <t>Семенов Саша</t>
+  </si>
+  <si>
+    <t>Ивлев Никита</t>
+  </si>
+  <si>
+    <t>Краснов Артем</t>
+  </si>
+  <si>
+    <t>Толстолыткин Влад</t>
+  </si>
+  <si>
+    <t>Олейник Света</t>
+  </si>
+  <si>
+    <t>Леонидова Ксюша</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ДМИТРИЕВ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Роман Юрьевич</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-744-70-02</t>
+  </si>
+  <si>
+    <t>Петренко Игнат</t>
+  </si>
+  <si>
+    <t>Кривко Дима</t>
+  </si>
+  <si>
+    <t>Олеся степина</t>
+  </si>
+  <si>
+    <t>Токарев Илья</t>
+  </si>
+  <si>
+    <t>Благий Вова</t>
+  </si>
+  <si>
+    <t>Дима Данильченко</t>
+  </si>
+  <si>
+    <t>КУдрин Илья</t>
+  </si>
+  <si>
+    <t>Марк Сучков</t>
+  </si>
+  <si>
+    <t>Олег Романов</t>
+  </si>
+  <si>
+    <t>Разумников Илья</t>
+  </si>
+  <si>
+    <t>Даня Григорян</t>
+  </si>
+  <si>
+    <t>Петров Антон</t>
+  </si>
+  <si>
+    <t>Ваня Санников</t>
+  </si>
+  <si>
+    <t>Паша Машаров</t>
+  </si>
+  <si>
+    <t>Леонтьев Артем</t>
+  </si>
+  <si>
+    <t>МАксим Трохачев</t>
+  </si>
+  <si>
+    <t>Тутов Станислав</t>
+  </si>
+  <si>
+    <t>Давыдов Вадим</t>
+  </si>
+  <si>
+    <t>Земцов Артем</t>
+  </si>
+  <si>
+    <t>Настя Приставка</t>
+  </si>
+  <si>
+    <t>Михалев Паша</t>
+  </si>
+  <si>
+    <t>Миша Блинков</t>
+  </si>
+  <si>
+    <t>Резниченко Олег</t>
+  </si>
+  <si>
+    <t>Курилова Настя</t>
+  </si>
+  <si>
+    <t>Кабанов Саша</t>
+  </si>
+  <si>
+    <t>Настя Блинкова</t>
+  </si>
+  <si>
+    <t>Бебенин Борис Александрович</t>
+  </si>
+  <si>
+    <t>Антон Клещев</t>
+  </si>
+  <si>
+    <t>Игнашин Максим</t>
+  </si>
+  <si>
+    <t>Лаптев Сергей</t>
+  </si>
+  <si>
+    <t>Шестов Стас</t>
+  </si>
+  <si>
+    <t>Растворов Кирилл</t>
+  </si>
+  <si>
+    <t>Новосело Дима</t>
+  </si>
+  <si>
+    <t>Мирзаева Элина</t>
+  </si>
+  <si>
+    <t>Кривенцов Илья</t>
+  </si>
+  <si>
+    <t>Баранов Олег</t>
+  </si>
+  <si>
+    <t>Костя Анисимов</t>
+  </si>
+  <si>
+    <t>Алексей Орлов</t>
+  </si>
+  <si>
+    <t>Лера Садовникова</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">САДОВНИКОВ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Дмитрий Васильевич</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-543-26-64</t>
+  </si>
+  <si>
+    <t>Лера Жена</t>
+  </si>
+  <si>
+    <t>+79782487684</t>
+  </si>
+  <si>
+    <t>Астапкович Дима</t>
+  </si>
+  <si>
+    <t>Евгений Надточеев</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ЯКОВЛЕВ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Константин</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Николаевич</t>
+    </r>
+  </si>
+  <si>
+    <t>8-978-296-52-77</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ДУДНИКОВ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Narrow"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Андрей Николаевич</t>
+    </r>
+  </si>
+  <si>
+    <t>8-910-744-87-55</t>
+  </si>
+  <si>
+    <t>Даша Сестра</t>
+  </si>
+  <si>
+    <t>Дима Павлов</t>
+  </si>
+  <si>
+    <t>Лиза</t>
+  </si>
+  <si>
+    <t>Ростик</t>
   </si>
 </sst>
 </file>
@@ -638,23 +1404,16 @@
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_-* #\ ##0_-;\-* #\ ##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #\ ##0\ &quot;₽&quot;_-;\-* #\ ##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #\ ##0.00\ &quot;₽&quot;_-;\-* #\ ##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="[$-419]d\ mmmm\ yyyy\ &quot;r.&quot;;@"/>
-    <numFmt numFmtId="180" formatCode="_-* #\ ##0.00_-;\-* #\ ##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #\ ##0.00_-;\-* #\ ##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #\ ##0.00\ &quot;₽&quot;_-;\-* #\ ##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="[$-419]d\ mmmm\ yyyy\ &quot;r.&quot;;@"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -666,7 +1425,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -679,8 +1438,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -691,30 +1458,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -734,8 +1477,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -774,6 +1532,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -788,8 +1553,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -801,6 +1567,13 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial Narrow"/>
@@ -822,7 +1595,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -834,13 +1625,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -852,31 +1691,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -894,19 +1715,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -918,25 +1751,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -948,61 +1769,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1031,17 +1804,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1049,8 +1816,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1105,11 +1872,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1131,52 +1904,55 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1185,94 +1961,91 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1280,10 +2053,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1605,8 +2379,8 @@
   <sheetPr/>
   <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1641,7 +2415,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3">
-        <v>19455</v>
+        <v>19377</v>
       </c>
       <c r="C3" s="4"/>
     </row>
@@ -1650,7 +2424,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>24202</v>
+        <v>24143</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -1670,7 +2444,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="3">
-        <v>24933</v>
+        <v>24937</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>9</v>
@@ -1942,393 +2716,753 @@
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="2"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="4"/>
+      <c r="A32" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="3">
+        <v>31824</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="4"/>
+      <c r="A33" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="3">
+        <v>32034</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="2"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="4"/>
+      <c r="A34" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="3">
+        <v>32045</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="2"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="4"/>
+      <c r="A35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="3">
+        <v>32612</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="2"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="4"/>
+      <c r="A36" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="3">
+        <v>32767</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="2"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="4"/>
+      <c r="A37" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="3">
+        <v>32767</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="2"/>
-      <c r="B38" s="3"/>
+      <c r="A38" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="3">
+        <v>33121</v>
+      </c>
       <c r="C38" s="4"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="2"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="4"/>
+      <c r="A39" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="3">
+        <v>33295</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="2"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="4"/>
+      <c r="A40" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="3">
+        <v>33476</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="2"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="4"/>
+      <c r="A41" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="3">
+        <v>33540</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="2"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="4"/>
+      <c r="A42" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" s="3">
+        <v>34063</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="2"/>
-      <c r="B43" s="3"/>
+      <c r="A43" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" s="3">
+        <v>34381</v>
+      </c>
       <c r="C43" s="4"/>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="2"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="4"/>
+      <c r="A44" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" s="3">
+        <v>34451</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="2"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="4"/>
+      <c r="A45" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" s="3">
+        <v>34505</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="2"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="4"/>
+      <c r="A46" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" s="3">
+        <v>34550</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="2"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="4"/>
+      <c r="A47" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47" s="3">
+        <v>34710</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="2"/>
-      <c r="B48" s="3"/>
+      <c r="A48" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" s="3">
+        <v>34735</v>
+      </c>
       <c r="C48" s="4"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="2"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="4"/>
+      <c r="A49" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="3">
+        <v>34834</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="2"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="4"/>
+      <c r="A50" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="3">
+        <v>34837</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="2"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="4"/>
+      <c r="A51" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B51" s="3">
+        <v>34856</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="2"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="4"/>
+      <c r="A52" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" s="3">
+        <v>34930</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="2"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="4"/>
+      <c r="A53" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B53" s="3">
+        <v>34997</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="2"/>
-      <c r="B54" s="3"/>
+      <c r="A54" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" s="3">
+        <v>35081</v>
+      </c>
       <c r="C54" s="4"/>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="2"/>
-      <c r="B55" s="3"/>
+      <c r="A55" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B55" s="3">
+        <v>35082</v>
+      </c>
       <c r="C55" s="4"/>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="2"/>
-      <c r="B56" s="3"/>
+      <c r="A56" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" s="3">
+        <v>35102</v>
+      </c>
       <c r="C56" s="4"/>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="2"/>
-      <c r="B57" s="3"/>
+      <c r="A57" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B57" s="3">
+        <v>35102</v>
+      </c>
       <c r="C57" s="4"/>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="2"/>
-      <c r="B58" s="3"/>
+      <c r="A58" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B58" s="3">
+        <v>35103</v>
+      </c>
       <c r="C58" s="4"/>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="2"/>
-      <c r="B59" s="3"/>
+      <c r="A59" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B59" s="3">
+        <v>35103</v>
+      </c>
       <c r="C59" s="4"/>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="2"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="4"/>
+      <c r="A60" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B60" s="3">
+        <v>35110</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="2"/>
-      <c r="B61" s="3"/>
+      <c r="A61" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B61" s="3">
+        <v>35121</v>
+      </c>
       <c r="C61" s="4"/>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="2"/>
-      <c r="B62" s="3"/>
+      <c r="A62" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B62" s="3">
+        <v>35143</v>
+      </c>
       <c r="C62" s="4"/>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="2"/>
-      <c r="B63" s="3"/>
+      <c r="A63" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B63" s="3">
+        <v>35149</v>
+      </c>
       <c r="C63" s="4"/>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="2"/>
-      <c r="B64" s="3"/>
+      <c r="A64" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B64" s="3">
+        <v>35153</v>
+      </c>
       <c r="C64" s="4"/>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="2"/>
-      <c r="B65" s="3"/>
+      <c r="A65" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B65" s="3">
+        <v>35154</v>
+      </c>
       <c r="C65" s="4"/>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="2"/>
-      <c r="B66" s="3"/>
+      <c r="A66" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B66" s="3">
+        <v>35156</v>
+      </c>
       <c r="C66" s="4"/>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="2"/>
-      <c r="B67" s="3"/>
+      <c r="A67" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B67" s="3">
+        <v>35164</v>
+      </c>
       <c r="C67" s="4"/>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="2"/>
-      <c r="B68" s="3"/>
+      <c r="A68" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B68" s="3">
+        <v>35173</v>
+      </c>
       <c r="C68" s="4"/>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="2"/>
-      <c r="B69" s="3"/>
+      <c r="A69" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B69" s="3">
+        <v>35181</v>
+      </c>
       <c r="C69" s="4"/>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="2"/>
-      <c r="B70" s="3"/>
+      <c r="A70" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B70" s="3">
+        <v>35186</v>
+      </c>
       <c r="C70" s="4"/>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="2"/>
-      <c r="B71" s="3"/>
+      <c r="A71" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B71" s="3">
+        <v>35195</v>
+      </c>
       <c r="C71" s="4"/>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="2"/>
-      <c r="B72" s="3"/>
+      <c r="A72" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B72" s="3">
+        <v>35213</v>
+      </c>
       <c r="C72" s="4"/>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="2"/>
-      <c r="B73" s="3"/>
+      <c r="A73" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B73" s="3">
+        <v>35225</v>
+      </c>
       <c r="C73" s="4"/>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="2"/>
-      <c r="B74" s="3"/>
+      <c r="A74" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B74" s="3">
+        <v>35243</v>
+      </c>
       <c r="C74" s="4"/>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="2"/>
-      <c r="B75" s="3"/>
+      <c r="A75" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B75" s="3">
+        <v>35252</v>
+      </c>
       <c r="C75" s="4"/>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="2"/>
-      <c r="B76" s="3"/>
+      <c r="A76" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B76" s="3">
+        <v>35264</v>
+      </c>
       <c r="C76" s="4"/>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="2"/>
-      <c r="B77" s="3"/>
+      <c r="A77" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B77" s="3">
+        <v>35264</v>
+      </c>
       <c r="C77" s="4"/>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="2"/>
-      <c r="B78" s="3"/>
+      <c r="A78" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B78" s="3">
+        <v>35265</v>
+      </c>
       <c r="C78" s="4"/>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="2"/>
-      <c r="B79" s="3"/>
+      <c r="A79" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B79" s="3">
+        <v>35268</v>
+      </c>
       <c r="C79" s="4"/>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" s="2"/>
-      <c r="B80" s="3"/>
+      <c r="A80" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B80" s="3">
+        <v>35270</v>
+      </c>
       <c r="C80" s="4"/>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="2"/>
-      <c r="B81" s="3"/>
+      <c r="A81" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B81" s="3">
+        <v>35307</v>
+      </c>
       <c r="C81" s="4"/>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="2"/>
-      <c r="B82" s="3"/>
+      <c r="A82" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B82" s="3">
+        <v>35312</v>
+      </c>
       <c r="C82" s="4"/>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="2"/>
-      <c r="B83" s="3"/>
+      <c r="A83" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B83" s="3">
+        <v>35317</v>
+      </c>
       <c r="C83" s="4"/>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" s="2"/>
-      <c r="B84" s="3"/>
+      <c r="A84" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B84" s="3">
+        <v>35331</v>
+      </c>
       <c r="C84" s="4"/>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="2"/>
-      <c r="B85" s="3"/>
+      <c r="A85" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B85" s="3">
+        <v>35334</v>
+      </c>
       <c r="C85" s="4"/>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="2"/>
-      <c r="B86" s="3"/>
+      <c r="A86" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B86" s="3">
+        <v>35338</v>
+      </c>
       <c r="C86" s="4"/>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="2"/>
-      <c r="B87" s="3"/>
+      <c r="A87" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B87" s="3">
+        <v>35339</v>
+      </c>
       <c r="C87" s="4"/>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="2"/>
-      <c r="B88" s="3"/>
+      <c r="A88" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B88" s="3">
+        <v>35339</v>
+      </c>
       <c r="C88" s="4"/>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="2"/>
-      <c r="B89" s="3"/>
+      <c r="A89" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B89" s="3">
+        <v>35344</v>
+      </c>
       <c r="C89" s="4"/>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" s="2"/>
-      <c r="B90" s="3"/>
+      <c r="A90" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B90" s="3">
+        <v>35345</v>
+      </c>
       <c r="C90" s="4"/>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="2"/>
-      <c r="B91" s="3"/>
+      <c r="A91" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B91" s="3">
+        <v>35360</v>
+      </c>
       <c r="C91" s="4"/>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" s="2"/>
-      <c r="B92" s="3"/>
+      <c r="A92" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B92" s="3">
+        <v>35374</v>
+      </c>
       <c r="C92" s="4"/>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="2"/>
-      <c r="B93" s="3"/>
+      <c r="A93" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B93" s="3">
+        <v>35376</v>
+      </c>
       <c r="C93" s="4"/>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="2"/>
-      <c r="B94" s="3"/>
+      <c r="A94" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B94" s="3">
+        <v>35386</v>
+      </c>
       <c r="C94" s="4"/>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="2"/>
-      <c r="B95" s="3"/>
+      <c r="A95" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B95" s="3">
+        <v>35401</v>
+      </c>
       <c r="C95" s="4"/>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="2"/>
-      <c r="B96" s="3"/>
+      <c r="A96" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B96" s="3">
+        <v>35417</v>
+      </c>
       <c r="C96" s="4"/>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="2"/>
-      <c r="B97" s="3"/>
+      <c r="A97" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B97" s="3">
+        <v>35440</v>
+      </c>
       <c r="C97" s="2"/>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="2"/>
-      <c r="B98" s="3"/>
+      <c r="A98" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B98" s="3">
+        <v>35453</v>
+      </c>
       <c r="C98" s="4"/>
     </row>
     <row r="99" spans="1:3">
-      <c r="A99" s="2"/>
-      <c r="B99" s="3"/>
+      <c r="A99" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B99" s="3">
+        <v>35463</v>
+      </c>
       <c r="C99" s="4"/>
     </row>
     <row r="100" spans="1:3">
-      <c r="A100" s="2"/>
-      <c r="B100" s="3"/>
-      <c r="C100" s="4"/>
+      <c r="A100" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B100" s="3">
+        <v>35545</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="101" spans="1:3">
-      <c r="A101" s="2"/>
-      <c r="B101" s="3"/>
-      <c r="C101" s="4"/>
+      <c r="A101" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B101" s="3">
+        <v>35601</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="102" spans="1:3">
-      <c r="A102" s="2"/>
-      <c r="B102" s="3"/>
+      <c r="A102" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B102" s="3">
+        <v>35643</v>
+      </c>
       <c r="C102" s="4"/>
     </row>
     <row r="103" spans="1:3">
-      <c r="A103" s="2"/>
-      <c r="B103" s="3"/>
+      <c r="A103" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B103" s="3">
+        <v>35805</v>
+      </c>
       <c r="C103" s="4"/>
     </row>
     <row r="104" spans="1:3">
-      <c r="A104" s="2"/>
-      <c r="B104" s="3"/>
-      <c r="C104" s="4"/>
+      <c r="A104" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B104" s="3">
+        <v>35845</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="105" spans="1:3">
-      <c r="A105" s="2"/>
-      <c r="B105" s="3"/>
-      <c r="C105" s="4"/>
+      <c r="A105" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B105" s="3">
+        <v>35955</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="106" spans="1:3">
-      <c r="A106" s="2"/>
-      <c r="B106" s="3"/>
+      <c r="A106" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B106" s="3">
+        <v>36741</v>
+      </c>
       <c r="C106" s="4"/>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" s="2"/>
-      <c r="B107" s="3"/>
+      <c r="A107" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B107" s="3">
+        <v>36836</v>
+      </c>
       <c r="C107" s="4"/>
     </row>
     <row r="108" spans="1:3">
-      <c r="A108" s="2"/>
-      <c r="B108" s="3"/>
+      <c r="A108" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B108" s="3">
+        <v>39597</v>
+      </c>
       <c r="C108" s="4"/>
     </row>
     <row r="109" spans="1:3">
-      <c r="A109" s="2"/>
-      <c r="B109" s="3"/>
+      <c r="A109" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B109" s="3">
+        <v>40210</v>
+      </c>
       <c r="C109" s="4"/>
     </row>
     <row r="110" spans="2:3">

</xml_diff>